<commit_message>
Expanded Address use valueset
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cbs-patient.xlsx
+++ b/output/StructureDefinition-cbs-patient.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="522">
   <si>
     <t>Path</t>
   </si>
@@ -925,10 +925,7 @@
     <t>home</t>
   </si>
   <si>
-    <t>The use of an address.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/address-use|4.0.1</t>
+    <t>http://cbsig.chai.gatech.edu/output/ValueSet/CBSAddressUseVS</t>
   </si>
   <si>
     <t>Address.use</t>
@@ -1204,9 +1201,6 @@
   </si>
   <si>
     <t>Usual-Residence</t>
-  </si>
-  <si>
-    <t>http://cbsig.chai.gatech.edu/output/ValueSet/CBSAddressUseVS</t>
   </si>
   <si>
     <t xml:space="preserve">Zip
@@ -6143,29 +6137,27 @@
       <c r="W38" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="X38" t="s" s="2">
+      <c r="X38" s="2"/>
+      <c r="Y38" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="Y38" t="s" s="2">
+      <c r="Z38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE38" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="Z38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE38" t="s" s="2">
-        <v>291</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>42</v>
@@ -6180,16 +6172,16 @@
         <v>63</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL38" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM38" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM38" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>44</v>
@@ -6197,7 +6189,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6223,13 +6215,13 @@
         <v>71</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -6243,7 +6235,7 @@
         <v>44</v>
       </c>
       <c r="S39" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T39" t="s" s="2">
         <v>44</v>
@@ -6258,28 +6250,28 @@
         <v>171</v>
       </c>
       <c r="X39" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="Y39" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="Y39" t="s" s="2">
+      <c r="Z39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE39" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>42</v>
@@ -6294,7 +6286,7 @@
         <v>63</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>44</v>
@@ -6303,7 +6295,7 @@
         <v>44</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>44</v>
@@ -6311,7 +6303,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6337,16 +6329,16 @@
         <v>53</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>44</v>
@@ -6359,43 +6351,43 @@
         <v>44</v>
       </c>
       <c r="S40" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="T40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE40" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="T40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>42</v>
@@ -6410,16 +6402,16 @@
         <v>63</v>
       </c>
       <c r="AJ40" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>311</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>44</v>
@@ -6427,7 +6419,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6453,10 +6445,10 @@
         <v>53</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6471,43 +6463,43 @@
         <v>44</v>
       </c>
       <c r="S41" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE41" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>42</v>
@@ -6522,16 +6514,16 @@
         <v>63</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>44</v>
@@ -6539,7 +6531,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6565,10 +6557,10 @@
         <v>53</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6651,7 +6643,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6761,10 +6753,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="B44" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="B44" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="C44" t="s" s="2">
         <v>44</v>
@@ -6786,13 +6778,13 @@
         <v>44</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6858,7 +6850,7 @@
         <v>102</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>44</v>
@@ -6875,7 +6867,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6901,10 +6893,10 @@
         <v>53</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>328</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6928,34 +6920,34 @@
         <v>44</v>
       </c>
       <c r="V45" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE45" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="W45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD45" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE45" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>42</v>
@@ -6987,11 +6979,11 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -7013,10 +7005,10 @@
         <v>53</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -7031,43 +7023,43 @@
         <v>44</v>
       </c>
       <c r="S46" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE46" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="T46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>42</v>
@@ -7082,16 +7074,16 @@
         <v>63</v>
       </c>
       <c r="AJ46" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="AK46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL46" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM46" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>44</v>
@@ -7099,11 +7091,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -7125,13 +7117,13 @@
         <v>53</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -7145,43 +7137,43 @@
         <v>44</v>
       </c>
       <c r="S47" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE47" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="T47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>42</v>
@@ -7196,16 +7188,16 @@
         <v>63</v>
       </c>
       <c r="AJ47" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM47" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="AK47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>44</v>
@@ -7213,11 +7205,11 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7239,10 +7231,10 @@
         <v>53</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -7293,7 +7285,7 @@
         <v>44</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>42</v>
@@ -7308,16 +7300,16 @@
         <v>63</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM48" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>44</v>
@@ -7325,11 +7317,11 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7351,10 +7343,10 @@
         <v>53</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>358</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>359</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -7369,43 +7361,43 @@
         <v>44</v>
       </c>
       <c r="S49" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE49" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="T49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE49" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>42</v>
@@ -7420,16 +7412,16 @@
         <v>63</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM49" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AK49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL49" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>44</v>
@@ -7437,7 +7429,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7463,13 +7455,13 @@
         <v>53</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7519,7 +7511,7 @@
         <v>44</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>42</v>
@@ -7534,16 +7526,16 @@
         <v>63</v>
       </c>
       <c r="AJ50" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL50" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>44</v>
@@ -7551,7 +7543,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7577,14 +7569,14 @@
         <v>203</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>44</v>
@@ -7597,43 +7589,43 @@
         <v>44</v>
       </c>
       <c r="S51" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="T51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE51" t="s" s="2">
         <v>375</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>42</v>
@@ -7648,16 +7640,16 @@
         <v>63</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AK51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL51" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM51" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>44</v>
@@ -7668,7 +7660,7 @@
         <v>271</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C52" t="s" s="2">
         <v>44</v>
@@ -8054,7 +8046,7 @@
         <v>44</v>
       </c>
       <c r="R55" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="S55" t="s" s="2">
         <v>288</v>
@@ -8073,7 +8065,7 @@
       </c>
       <c r="X55" s="2"/>
       <c r="Y55" t="s" s="2">
-        <v>380</v>
+        <v>289</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>44</v>
@@ -8091,7 +8083,7 @@
         <v>44</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>42</v>
@@ -8106,16 +8098,16 @@
         <v>63</v>
       </c>
       <c r="AJ55" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM55" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>44</v>
@@ -8123,7 +8115,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8149,13 +8141,13 @@
         <v>71</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -8169,7 +8161,7 @@
         <v>44</v>
       </c>
       <c r="S56" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T56" t="s" s="2">
         <v>44</v>
@@ -8184,28 +8176,28 @@
         <v>171</v>
       </c>
       <c r="X56" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="Y56" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="Y56" t="s" s="2">
+      <c r="Z56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE56" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>42</v>
@@ -8220,7 +8212,7 @@
         <v>63</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>44</v>
@@ -8229,7 +8221,7 @@
         <v>44</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>44</v>
@@ -8237,7 +8229,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8263,16 +8255,16 @@
         <v>53</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>44</v>
@@ -8285,43 +8277,43 @@
         <v>44</v>
       </c>
       <c r="S57" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE57" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="T57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE57" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -8336,16 +8328,16 @@
         <v>63</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM57" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>311</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>44</v>
@@ -8353,7 +8345,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8379,10 +8371,10 @@
         <v>53</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -8397,43 +8389,43 @@
         <v>44</v>
       </c>
       <c r="S58" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE58" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="T58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE58" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>42</v>
@@ -8448,16 +8440,16 @@
         <v>63</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AK58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM58" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>44</v>
@@ -8465,11 +8457,11 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -8491,10 +8483,10 @@
         <v>53</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8509,43 +8501,43 @@
         <v>44</v>
       </c>
       <c r="S59" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE59" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="T59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE59" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>42</v>
@@ -8560,16 +8552,16 @@
         <v>63</v>
       </c>
       <c r="AJ59" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL59" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM59" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="AK59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL59" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>44</v>
@@ -8577,11 +8569,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8603,13 +8595,13 @@
         <v>53</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -8623,43 +8615,43 @@
         <v>44</v>
       </c>
       <c r="S60" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE60" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="T60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE60" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8674,16 +8666,16 @@
         <v>63</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM60" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>44</v>
@@ -8691,11 +8683,11 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -8717,10 +8709,10 @@
         <v>53</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8771,7 +8763,7 @@
         <v>44</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8786,16 +8778,16 @@
         <v>63</v>
       </c>
       <c r="AJ61" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM61" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>44</v>
@@ -8803,11 +8795,11 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8829,10 +8821,10 @@
         <v>53</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8847,43 +8839,43 @@
         <v>44</v>
       </c>
       <c r="S62" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE62" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="T62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>42</v>
@@ -8898,16 +8890,16 @@
         <v>63</v>
       </c>
       <c r="AJ62" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM62" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>44</v>
@@ -8915,7 +8907,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8941,13 +8933,13 @@
         <v>53</v>
       </c>
       <c r="K63" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L63" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="L63" t="s" s="2">
+      <c r="M63" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8997,7 +8989,7 @@
         <v>44</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>42</v>
@@ -9012,16 +9004,16 @@
         <v>63</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AK63" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL63" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM63" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>44</v>
@@ -9029,7 +9021,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9055,14 +9047,14 @@
         <v>203</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>44</v>
@@ -9075,43 +9067,43 @@
         <v>44</v>
       </c>
       <c r="S64" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="T64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE64" t="s" s="2">
         <v>375</v>
-      </c>
-      <c r="T64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE64" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>42</v>
@@ -9126,16 +9118,16 @@
         <v>63</v>
       </c>
       <c r="AJ64" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL64" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM64" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>44</v>
@@ -9146,7 +9138,7 @@
         <v>271</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C65" t="s" s="2">
         <v>44</v>
@@ -9532,7 +9524,7 @@
         <v>44</v>
       </c>
       <c r="R68" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S68" t="s" s="2">
         <v>288</v>
@@ -9551,7 +9543,7 @@
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" t="s" s="2">
-        <v>380</v>
+        <v>289</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>44</v>
@@ -9569,7 +9561,7 @@
         <v>44</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>42</v>
@@ -9584,16 +9576,16 @@
         <v>63</v>
       </c>
       <c r="AJ68" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL68" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM68" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>44</v>
@@ -9601,7 +9593,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9627,13 +9619,13 @@
         <v>71</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="M69" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
@@ -9647,7 +9639,7 @@
         <v>44</v>
       </c>
       <c r="S69" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T69" t="s" s="2">
         <v>44</v>
@@ -9662,28 +9654,28 @@
         <v>171</v>
       </c>
       <c r="X69" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="Y69" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="Y69" t="s" s="2">
+      <c r="Z69" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE69" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>42</v>
@@ -9698,7 +9690,7 @@
         <v>63</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AK69" t="s" s="2">
         <v>44</v>
@@ -9707,7 +9699,7 @@
         <v>44</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>44</v>
@@ -9715,7 +9707,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9741,16 +9733,16 @@
         <v>53</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="M70" t="s" s="2">
+      <c r="N70" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>44</v>
@@ -9763,43 +9755,43 @@
         <v>44</v>
       </c>
       <c r="S70" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="T70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE70" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>42</v>
@@ -9814,16 +9806,16 @@
         <v>63</v>
       </c>
       <c r="AJ70" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL70" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM70" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>311</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>44</v>
@@ -9831,7 +9823,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9857,10 +9849,10 @@
         <v>53</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9875,43 +9867,43 @@
         <v>44</v>
       </c>
       <c r="S71" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE71" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>42</v>
@@ -9926,16 +9918,16 @@
         <v>63</v>
       </c>
       <c r="AJ71" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL71" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM71" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM71" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>44</v>
@@ -9943,11 +9935,11 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
@@ -9969,10 +9961,10 @@
         <v>53</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -9987,43 +9979,43 @@
         <v>44</v>
       </c>
       <c r="S72" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="T72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE72" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>42</v>
@@ -10038,16 +10030,16 @@
         <v>63</v>
       </c>
       <c r="AJ72" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AK72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL72" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM72" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM72" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>44</v>
@@ -10055,11 +10047,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -10081,13 +10073,13 @@
         <v>53</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="L73" t="s" s="2">
+      <c r="M73" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
@@ -10101,43 +10093,43 @@
         <v>44</v>
       </c>
       <c r="S73" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="T73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE73" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>42</v>
@@ -10152,16 +10144,16 @@
         <v>63</v>
       </c>
       <c r="AJ73" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM73" t="s" s="2">
         <v>347</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>44</v>
@@ -10169,11 +10161,11 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" t="s" s="2">
@@ -10195,10 +10187,10 @@
         <v>53</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -10249,7 +10241,7 @@
         <v>44</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>42</v>
@@ -10264,16 +10256,16 @@
         <v>63</v>
       </c>
       <c r="AJ74" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AK74" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL74" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM74" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>44</v>
@@ -10281,11 +10273,11 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
@@ -10307,10 +10299,10 @@
         <v>53</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -10325,43 +10317,43 @@
         <v>44</v>
       </c>
       <c r="S75" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="T75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE75" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>42</v>
@@ -10376,16 +10368,16 @@
         <v>63</v>
       </c>
       <c r="AJ75" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AK75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL75" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM75" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>44</v>
@@ -10393,7 +10385,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10419,13 +10411,13 @@
         <v>53</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="L76" t="s" s="2">
+      <c r="M76" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
@@ -10475,7 +10467,7 @@
         <v>44</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>42</v>
@@ -10490,16 +10482,16 @@
         <v>63</v>
       </c>
       <c r="AJ76" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AK76" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL76" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM76" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>44</v>
@@ -10507,7 +10499,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10533,14 +10525,14 @@
         <v>203</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>44</v>
@@ -10553,43 +10545,43 @@
         <v>44</v>
       </c>
       <c r="S77" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="T77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE77" t="s" s="2">
         <v>375</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>42</v>
@@ -10604,16 +10596,16 @@
         <v>63</v>
       </c>
       <c r="AJ77" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AK77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM77" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>44</v>
@@ -10621,7 +10613,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10647,14 +10639,14 @@
         <v>136</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="O78" t="s" s="2">
         <v>44</v>
@@ -10682,10 +10674,10 @@
         <v>139</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="Z78" t="s" s="2">
         <v>44</v>
@@ -10703,7 +10695,7 @@
         <v>44</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>42</v>
@@ -10718,16 +10710,16 @@
         <v>63</v>
       </c>
       <c r="AJ78" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AK78" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AL78" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM78" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>44</v>
@@ -10735,7 +10727,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10758,19 +10750,19 @@
         <v>44</v>
       </c>
       <c r="J79" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="K79" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L79" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="K79" t="s" s="2">
+      <c r="M79" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="L79" t="s" s="2">
+      <c r="N79" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>44</v>
@@ -10819,7 +10811,7 @@
         <v>44</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>42</v>
@@ -10834,7 +10826,7 @@
         <v>63</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>125</v>
@@ -10843,7 +10835,7 @@
         <v>44</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>44</v>
@@ -10851,7 +10843,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10874,19 +10866,19 @@
         <v>44</v>
       </c>
       <c r="J80" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="K80" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="L80" t="s" s="2">
         <v>402</v>
       </c>
-      <c r="K80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="N80" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>44</v>
@@ -10935,7 +10927,7 @@
         <v>44</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>42</v>
@@ -10950,7 +10942,7 @@
         <v>63</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>125</v>
@@ -10959,7 +10951,7 @@
         <v>44</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AN80" t="s" s="2">
         <v>44</v>
@@ -10967,7 +10959,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10990,19 +10982,19 @@
         <v>44</v>
       </c>
       <c r="J81" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="K81" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="L81" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="K81" t="s" s="2">
+      <c r="M81" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="L81" t="s" s="2">
+      <c r="N81" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="N81" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>44</v>
@@ -11051,7 +11043,7 @@
         <v>44</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>42</v>
@@ -11063,10 +11055,10 @@
         <v>44</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>125</v>
@@ -11083,7 +11075,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11195,7 +11187,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -11309,11 +11301,11 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
@@ -11335,10 +11327,10 @@
         <v>96</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M84" t="s" s="2">
         <v>150</v>
@@ -11393,7 +11385,7 @@
         <v>44</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>42</v>
@@ -11425,7 +11417,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11451,14 +11443,14 @@
         <v>136</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" t="s" s="2">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O85" t="s" s="2">
         <v>44</v>
@@ -11486,10 +11478,10 @@
         <v>139</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="Y85" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="Z85" t="s" s="2">
         <v>44</v>
@@ -11507,7 +11499,7 @@
         <v>44</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>42</v>
@@ -11522,7 +11514,7 @@
         <v>63</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>125</v>
@@ -11531,7 +11523,7 @@
         <v>44</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AN85" t="s" s="2">
         <v>44</v>
@@ -11539,7 +11531,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11565,14 +11557,14 @@
         <v>227</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>44</v>
@@ -11621,7 +11613,7 @@
         <v>44</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>42</v>
@@ -11645,7 +11637,7 @@
         <v>44</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AN86" t="s" s="2">
         <v>44</v>
@@ -11653,7 +11645,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11679,13 +11671,13 @@
         <v>236</v>
       </c>
       <c r="K87" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="L87" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="M87" t="s" s="2">
         <v>438</v>
-      </c>
-      <c r="L87" t="s" s="2">
-        <v>439</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="N87" t="s" s="2">
         <v>240</v>
@@ -11737,7 +11729,7 @@
         <v>44</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>42</v>
@@ -11761,7 +11753,7 @@
         <v>44</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AN87" t="s" s="2">
         <v>44</v>
@@ -11769,7 +11761,7 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11795,14 +11787,14 @@
         <v>272</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" t="s" s="2">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="O88" t="s" s="2">
         <v>44</v>
@@ -11851,7 +11843,7 @@
         <v>44</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>42</v>
@@ -11875,7 +11867,7 @@
         <v>44</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>44</v>
@@ -11883,7 +11875,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11912,11 +11904,11 @@
         <v>245</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="M89" s="2"/>
       <c r="N89" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="O89" t="s" s="2">
         <v>44</v>
@@ -11944,10 +11936,10 @@
         <v>171</v>
       </c>
       <c r="X89" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="Z89" t="s" s="2">
         <v>44</v>
@@ -11965,7 +11957,7 @@
         <v>44</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>42</v>
@@ -11989,7 +11981,7 @@
         <v>44</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>44</v>
@@ -11997,7 +11989,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -12023,14 +12015,14 @@
         <v>210</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" t="s" s="2">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O90" t="s" s="2">
         <v>44</v>
@@ -12079,7 +12071,7 @@
         <v>44</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>42</v>
@@ -12088,13 +12080,13 @@
         <v>51</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="AK90" t="s" s="2">
         <v>125</v>
@@ -12103,7 +12095,7 @@
         <v>44</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>44</v>
@@ -12111,7 +12103,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -12137,10 +12129,10 @@
         <v>203</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -12191,7 +12183,7 @@
         <v>44</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>42</v>
@@ -12206,7 +12198,7 @@
         <v>63</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="AK91" t="s" s="2">
         <v>125</v>
@@ -12223,7 +12215,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12246,19 +12238,19 @@
         <v>44</v>
       </c>
       <c r="J92" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K92" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="M92" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="L92" t="s" s="2">
+      <c r="N92" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="M92" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="N92" t="s" s="2">
-        <v>468</v>
       </c>
       <c r="O92" t="s" s="2">
         <v>44</v>
@@ -12307,7 +12299,7 @@
         <v>44</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>42</v>
@@ -12322,10 +12314,10 @@
         <v>63</v>
       </c>
       <c r="AJ92" t="s" s="2">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>44</v>
@@ -12339,7 +12331,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -12451,7 +12443,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -12565,11 +12557,11 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" t="s" s="2">
@@ -12591,10 +12583,10 @@
         <v>96</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M95" t="s" s="2">
         <v>150</v>
@@ -12649,7 +12641,7 @@
         <v>44</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>42</v>
@@ -12681,7 +12673,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -12707,16 +12699,16 @@
         <v>136</v>
       </c>
       <c r="K96" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="M96" t="s" s="2">
         <v>475</v>
       </c>
-      <c r="L96" t="s" s="2">
+      <c r="N96" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="M96" t="s" s="2">
-        <v>477</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>478</v>
       </c>
       <c r="O96" t="s" s="2">
         <v>44</v>
@@ -12765,7 +12757,7 @@
         <v>44</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>51</v>
@@ -12780,16 +12772,16 @@
         <v>63</v>
       </c>
       <c r="AJ96" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="AK96" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM96" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="AK96" t="s" s="2">
-        <v>480</v>
-      </c>
-      <c r="AL96" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM96" t="s" s="2">
-        <v>481</v>
       </c>
       <c r="AN96" t="s" s="2">
         <v>44</v>
@@ -12797,7 +12789,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -12823,16 +12815,16 @@
         <v>218</v>
       </c>
       <c r="K97" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="M97" t="s" s="2">
         <v>483</v>
       </c>
-      <c r="L97" t="s" s="2">
+      <c r="N97" t="s" s="2">
         <v>484</v>
-      </c>
-      <c r="M97" t="s" s="2">
-        <v>485</v>
-      </c>
-      <c r="N97" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="O97" t="s" s="2">
         <v>44</v>
@@ -12881,7 +12873,7 @@
         <v>44</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="AF97" t="s" s="2">
         <v>42</v>
@@ -12896,16 +12888,16 @@
         <v>63</v>
       </c>
       <c r="AJ97" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AL97" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM97" t="s" s="2">
         <v>487</v>
-      </c>
-      <c r="AK97" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="AL97" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM97" t="s" s="2">
-        <v>489</v>
       </c>
       <c r="AN97" t="s" s="2">
         <v>44</v>
@@ -12913,11 +12905,11 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" t="s" s="2">
@@ -12936,16 +12928,16 @@
         <v>44</v>
       </c>
       <c r="J98" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="K98" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="L98" t="s" s="2">
         <v>492</v>
       </c>
-      <c r="K98" t="s" s="2">
+      <c r="M98" t="s" s="2">
         <v>493</v>
-      </c>
-      <c r="L98" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="M98" t="s" s="2">
-        <v>495</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" t="s" s="2">
@@ -12995,7 +12987,7 @@
         <v>44</v>
       </c>
       <c r="AE98" t="s" s="2">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="AF98" t="s" s="2">
         <v>42</v>
@@ -13010,7 +13002,7 @@
         <v>63</v>
       </c>
       <c r="AJ98" t="s" s="2">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AK98" t="s" s="2">
         <v>125</v>
@@ -13019,7 +13011,7 @@
         <v>44</v>
       </c>
       <c r="AM98" t="s" s="2">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AN98" t="s" s="2">
         <v>44</v>
@@ -13027,7 +13019,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -13053,16 +13045,16 @@
         <v>210</v>
       </c>
       <c r="K99" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="L99" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="M99" t="s" s="2">
         <v>499</v>
       </c>
-      <c r="L99" t="s" s="2">
+      <c r="N99" t="s" s="2">
         <v>500</v>
-      </c>
-      <c r="M99" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="N99" t="s" s="2">
-        <v>502</v>
       </c>
       <c r="O99" t="s" s="2">
         <v>44</v>
@@ -13111,7 +13103,7 @@
         <v>44</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>42</v>
@@ -13126,10 +13118,10 @@
         <v>63</v>
       </c>
       <c r="AJ99" t="s" s="2">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AL99" t="s" s="2">
         <v>44</v>
@@ -13143,7 +13135,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -13166,19 +13158,19 @@
         <v>52</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K100" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="L100" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="M100" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="L100" t="s" s="2">
+      <c r="N100" t="s" s="2">
         <v>506</v>
-      </c>
-      <c r="M100" t="s" s="2">
-        <v>507</v>
-      </c>
-      <c r="N100" t="s" s="2">
-        <v>508</v>
       </c>
       <c r="O100" t="s" s="2">
         <v>44</v>
@@ -13227,7 +13219,7 @@
         <v>44</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>42</v>
@@ -13242,7 +13234,7 @@
         <v>63</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="AK100" t="s" s="2">
         <v>125</v>
@@ -13259,7 +13251,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13371,7 +13363,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13485,11 +13477,11 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" t="s" s="2">
@@ -13511,10 +13503,10 @@
         <v>96</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M103" t="s" s="2">
         <v>150</v>
@@ -13569,7 +13561,7 @@
         <v>44</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>42</v>
@@ -13601,7 +13593,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -13624,16 +13616,16 @@
         <v>52</v>
       </c>
       <c r="J104" t="s" s="2">
+        <v>512</v>
+      </c>
+      <c r="K104" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="L104" t="s" s="2">
         <v>514</v>
       </c>
-      <c r="K104" t="s" s="2">
+      <c r="M104" t="s" s="2">
         <v>515</v>
-      </c>
-      <c r="L104" t="s" s="2">
-        <v>516</v>
-      </c>
-      <c r="M104" t="s" s="2">
-        <v>517</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" t="s" s="2">
@@ -13683,7 +13675,7 @@
         <v>44</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>51</v>
@@ -13707,7 +13699,7 @@
         <v>44</v>
       </c>
       <c r="AM104" t="s" s="2">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AN104" t="s" s="2">
         <v>44</v>
@@ -13715,7 +13707,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13741,10 +13733,10 @@
         <v>71</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -13774,10 +13766,10 @@
         <v>171</v>
       </c>
       <c r="X105" t="s" s="2">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="Y105" t="s" s="2">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="Z105" t="s" s="2">
         <v>44</v>
@@ -13795,7 +13787,7 @@
         <v>44</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>51</v>
@@ -13810,7 +13802,7 @@
         <v>63</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="AK105" t="s" s="2">
         <v>125</v>

</xml_diff>

<commit_message>
Added new output files
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cbs-patient.xlsx
+++ b/output/StructureDefinition-cbs-patient.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3782" uniqueCount="524">
   <si>
     <t>Path</t>
   </si>
@@ -1201,6 +1201,12 @@
   </si>
   <si>
     <t>Usual-Residence</t>
+  </si>
+  <si>
+    <t>The use of an address.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/address-use|4.0.1</t>
   </si>
   <si>
     <t xml:space="preserve">Zip
@@ -8063,9 +8069,11 @@
       <c r="W55" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="X55" s="2"/>
+      <c r="X55" t="s" s="2">
+        <v>379</v>
+      </c>
       <c r="Y55" t="s" s="2">
-        <v>289</v>
+        <v>380</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>44</v>
@@ -8799,7 +8807,7 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
@@ -8821,7 +8829,7 @@
         <v>53</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="L62" t="s" s="2">
         <v>358</v>
@@ -9138,7 +9146,7 @@
         <v>271</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C65" t="s" s="2">
         <v>44</v>
@@ -9524,7 +9532,7 @@
         <v>44</v>
       </c>
       <c r="R68" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="S68" t="s" s="2">
         <v>288</v>
@@ -9541,9 +9549,11 @@
       <c r="W68" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="X68" s="2"/>
+      <c r="X68" t="s" s="2">
+        <v>379</v>
+      </c>
       <c r="Y68" t="s" s="2">
-        <v>289</v>
+        <v>380</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>44</v>
@@ -10277,7 +10287,7 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
@@ -10299,7 +10309,7 @@
         <v>53</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="L75" t="s" s="2">
         <v>358</v>
@@ -10613,7 +10623,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10639,14 +10649,14 @@
         <v>136</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="O78" t="s" s="2">
         <v>44</v>
@@ -10674,10 +10684,10 @@
         <v>139</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="Z78" t="s" s="2">
         <v>44</v>
@@ -10695,7 +10705,7 @@
         <v>44</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>42</v>
@@ -10710,16 +10720,16 @@
         <v>63</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>44</v>
@@ -10727,7 +10737,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10750,19 +10760,19 @@
         <v>44</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>44</v>
@@ -10811,7 +10821,7 @@
         <v>44</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>42</v>
@@ -10826,7 +10836,7 @@
         <v>63</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="AK79" t="s" s="2">
         <v>125</v>
@@ -10835,7 +10845,7 @@
         <v>44</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>44</v>
@@ -10843,7 +10853,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10866,19 +10876,19 @@
         <v>44</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>44</v>
@@ -10927,7 +10937,7 @@
         <v>44</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>42</v>
@@ -10942,7 +10952,7 @@
         <v>63</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>125</v>
@@ -10951,7 +10961,7 @@
         <v>44</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="AN80" t="s" s="2">
         <v>44</v>
@@ -10959,7 +10969,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10982,19 +10992,19 @@
         <v>44</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>44</v>
@@ -11043,7 +11053,7 @@
         <v>44</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>42</v>
@@ -11055,10 +11065,10 @@
         <v>44</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>125</v>
@@ -11075,7 +11085,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11187,7 +11197,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -11301,11 +11311,11 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
@@ -11327,10 +11337,10 @@
         <v>96</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M84" t="s" s="2">
         <v>150</v>
@@ -11385,7 +11395,7 @@
         <v>44</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>42</v>
@@ -11417,7 +11427,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11443,14 +11453,14 @@
         <v>136</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" t="s" s="2">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="O85" t="s" s="2">
         <v>44</v>
@@ -11478,10 +11488,10 @@
         <v>139</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="Y85" t="s" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="Z85" t="s" s="2">
         <v>44</v>
@@ -11499,7 +11509,7 @@
         <v>44</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>42</v>
@@ -11514,7 +11524,7 @@
         <v>63</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>125</v>
@@ -11523,7 +11533,7 @@
         <v>44</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="AN85" t="s" s="2">
         <v>44</v>
@@ -11531,7 +11541,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11557,14 +11567,14 @@
         <v>227</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" t="s" s="2">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>44</v>
@@ -11613,7 +11623,7 @@
         <v>44</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>42</v>
@@ -11637,7 +11647,7 @@
         <v>44</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="AN86" t="s" s="2">
         <v>44</v>
@@ -11645,7 +11655,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -11671,13 +11681,13 @@
         <v>236</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N87" t="s" s="2">
         <v>240</v>
@@ -11729,7 +11739,7 @@
         <v>44</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>42</v>
@@ -11753,7 +11763,7 @@
         <v>44</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="AN87" t="s" s="2">
         <v>44</v>
@@ -11761,7 +11771,7 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11787,14 +11797,14 @@
         <v>272</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="O88" t="s" s="2">
         <v>44</v>
@@ -11843,7 +11853,7 @@
         <v>44</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>42</v>
@@ -11867,7 +11877,7 @@
         <v>44</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>44</v>
@@ -11875,7 +11885,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11904,11 +11914,11 @@
         <v>245</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="M89" s="2"/>
       <c r="N89" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="O89" t="s" s="2">
         <v>44</v>
@@ -11936,10 +11946,10 @@
         <v>171</v>
       </c>
       <c r="X89" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="Z89" t="s" s="2">
         <v>44</v>
@@ -11957,7 +11967,7 @@
         <v>44</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>42</v>
@@ -11981,7 +11991,7 @@
         <v>44</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>44</v>
@@ -11989,7 +11999,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -12015,14 +12025,14 @@
         <v>210</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="O90" t="s" s="2">
         <v>44</v>
@@ -12071,7 +12081,7 @@
         <v>44</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>42</v>
@@ -12080,13 +12090,13 @@
         <v>51</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AK90" t="s" s="2">
         <v>125</v>
@@ -12095,7 +12105,7 @@
         <v>44</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>44</v>
@@ -12103,7 +12113,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -12129,10 +12139,10 @@
         <v>203</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -12183,7 +12193,7 @@
         <v>44</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>42</v>
@@ -12198,7 +12208,7 @@
         <v>63</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="AK91" t="s" s="2">
         <v>125</v>
@@ -12215,7 +12225,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12238,19 +12248,19 @@
         <v>44</v>
       </c>
       <c r="J92" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="N92" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="O92" t="s" s="2">
         <v>44</v>
@@ -12299,7 +12309,7 @@
         <v>44</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>42</v>
@@ -12314,10 +12324,10 @@
         <v>63</v>
       </c>
       <c r="AJ92" t="s" s="2">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>44</v>
@@ -12331,7 +12341,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -12443,7 +12453,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -12557,11 +12567,11 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" t="s" s="2">
@@ -12583,10 +12593,10 @@
         <v>96</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M95" t="s" s="2">
         <v>150</v>
@@ -12641,7 +12651,7 @@
         <v>44</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>42</v>
@@ -12673,7 +12683,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -12699,16 +12709,16 @@
         <v>136</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="N96" t="s" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="O96" t="s" s="2">
         <v>44</v>
@@ -12757,7 +12767,7 @@
         <v>44</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>51</v>
@@ -12772,16 +12782,16 @@
         <v>63</v>
       </c>
       <c r="AJ96" t="s" s="2">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="AK96" t="s" s="2">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="AL96" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM96" t="s" s="2">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="AN96" t="s" s="2">
         <v>44</v>
@@ -12789,7 +12799,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -12815,16 +12825,16 @@
         <v>218</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="N97" t="s" s="2">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="O97" t="s" s="2">
         <v>44</v>
@@ -12873,7 +12883,7 @@
         <v>44</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="AF97" t="s" s="2">
         <v>42</v>
@@ -12888,16 +12898,16 @@
         <v>63</v>
       </c>
       <c r="AJ97" t="s" s="2">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="AK97" t="s" s="2">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="AL97" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM97" t="s" s="2">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="AN97" t="s" s="2">
         <v>44</v>
@@ -12905,11 +12915,11 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" t="s" s="2">
@@ -12928,16 +12938,16 @@
         <v>44</v>
       </c>
       <c r="J98" t="s" s="2">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="M98" t="s" s="2">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" t="s" s="2">
@@ -12987,7 +12997,7 @@
         <v>44</v>
       </c>
       <c r="AE98" t="s" s="2">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="AF98" t="s" s="2">
         <v>42</v>
@@ -13002,7 +13012,7 @@
         <v>63</v>
       </c>
       <c r="AJ98" t="s" s="2">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="AK98" t="s" s="2">
         <v>125</v>
@@ -13011,7 +13021,7 @@
         <v>44</v>
       </c>
       <c r="AM98" t="s" s="2">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="AN98" t="s" s="2">
         <v>44</v>
@@ -13019,7 +13029,7 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
@@ -13045,16 +13055,16 @@
         <v>210</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="M99" t="s" s="2">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="N99" t="s" s="2">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="O99" t="s" s="2">
         <v>44</v>
@@ -13103,7 +13113,7 @@
         <v>44</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>42</v>
@@ -13118,10 +13128,10 @@
         <v>63</v>
       </c>
       <c r="AJ99" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="AL99" t="s" s="2">
         <v>44</v>
@@ -13135,7 +13145,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -13158,19 +13168,19 @@
         <v>52</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="O100" t="s" s="2">
         <v>44</v>
@@ -13219,7 +13229,7 @@
         <v>44</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>42</v>
@@ -13234,7 +13244,7 @@
         <v>63</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="AK100" t="s" s="2">
         <v>125</v>
@@ -13251,7 +13261,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13363,7 +13373,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13477,11 +13487,11 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" t="s" s="2">
@@ -13503,10 +13513,10 @@
         <v>96</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M103" t="s" s="2">
         <v>150</v>
@@ -13561,7 +13571,7 @@
         <v>44</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>42</v>
@@ -13593,7 +13603,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -13616,16 +13626,16 @@
         <v>52</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" t="s" s="2">
@@ -13675,7 +13685,7 @@
         <v>44</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>51</v>
@@ -13699,7 +13709,7 @@
         <v>44</v>
       </c>
       <c r="AM104" t="s" s="2">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="AN104" t="s" s="2">
         <v>44</v>
@@ -13707,7 +13717,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13733,10 +13743,10 @@
         <v>71</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -13766,28 +13776,28 @@
         <v>171</v>
       </c>
       <c r="X105" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="Y105" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="Z105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD105" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE105" t="s" s="2">
         <v>519</v>
-      </c>
-      <c r="Y105" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="Z105" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA105" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB105" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC105" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD105" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE105" t="s" s="2">
-        <v>517</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>51</v>
@@ -13802,7 +13812,7 @@
         <v>63</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="AK105" t="s" s="2">
         <v>125</v>

</xml_diff>